<commit_message>
fixing l ordre alphabetique d affichage de notes et ajouter genrate query a route
</commit_message>
<xml_diff>
--- a/data_excel/Notes_GINF2.xlsx
+++ b/data_excel/Notes_GINF2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP EliteBooK\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP EliteBooK\gestionEnsatXML\data_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1030,7 +1030,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A891" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A463" workbookViewId="0">
+      <selection activeCell="I476" sqref="I476"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1123,7 +1125,7 @@
         <v>203</v>
       </c>
       <c r="G4">
-        <v>13.45</v>
+        <v>13.954999999999901</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1192,7 +1194,7 @@
         <v>203</v>
       </c>
       <c r="G7">
-        <v>13.16</v>
+        <v>16.344999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1261,7 +1263,7 @@
         <v>203</v>
       </c>
       <c r="G10">
-        <v>13.52</v>
+        <v>10.774999999999901</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -1330,7 +1332,7 @@
         <v>203</v>
       </c>
       <c r="G13">
-        <v>14.19</v>
+        <v>14.484999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1399,7 +1401,7 @@
         <v>203</v>
       </c>
       <c r="G16">
-        <v>10.58</v>
+        <v>15.315</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1468,7 +1470,7 @@
         <v>203</v>
       </c>
       <c r="G19">
-        <v>11.59</v>
+        <v>15.93</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1537,7 +1539,7 @@
         <v>203</v>
       </c>
       <c r="G22">
-        <v>11.39</v>
+        <v>16.489999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1606,7 +1608,7 @@
         <v>203</v>
       </c>
       <c r="G25">
-        <v>18.09</v>
+        <v>13.1299999999999</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -1675,7 +1677,7 @@
         <v>203</v>
       </c>
       <c r="G28">
-        <v>14.96</v>
+        <v>12.65</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1744,7 +1746,7 @@
         <v>203</v>
       </c>
       <c r="G31">
-        <v>17.329999999999998</v>
+        <v>15.56</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -1813,7 +1815,7 @@
         <v>203</v>
       </c>
       <c r="G34">
-        <v>19</v>
+        <v>14.404999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1882,7 +1884,7 @@
         <v>203</v>
       </c>
       <c r="G37">
-        <v>14.31</v>
+        <v>11.425000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1951,7 +1953,7 @@
         <v>203</v>
       </c>
       <c r="G40">
-        <v>16.82</v>
+        <v>15.69</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -2020,7 +2022,7 @@
         <v>203</v>
       </c>
       <c r="G43">
-        <v>15.27</v>
+        <v>14.475</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -2089,7 +2091,7 @@
         <v>203</v>
       </c>
       <c r="G46">
-        <v>15.74</v>
+        <v>14.494999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -2158,7 +2160,7 @@
         <v>203</v>
       </c>
       <c r="G49">
-        <v>11.12</v>
+        <v>11.969999999999899</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
@@ -2227,7 +2229,7 @@
         <v>203</v>
       </c>
       <c r="G52">
-        <v>16.73</v>
+        <v>15.114999999999901</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -2296,7 +2298,7 @@
         <v>203</v>
       </c>
       <c r="G55">
-        <v>10.49</v>
+        <v>18.36</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -2365,7 +2367,7 @@
         <v>203</v>
       </c>
       <c r="G58">
-        <v>11.15</v>
+        <v>17.795000000000002</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -2434,7 +2436,7 @@
         <v>203</v>
       </c>
       <c r="G61">
-        <v>15.57</v>
+        <v>16.774999999999999</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -2503,7 +2505,7 @@
         <v>203</v>
       </c>
       <c r="G64">
-        <v>15.24</v>
+        <v>11.335000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -2572,7 +2574,7 @@
         <v>203</v>
       </c>
       <c r="G67">
-        <v>16.46</v>
+        <v>18.64</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -2641,7 +2643,7 @@
         <v>203</v>
       </c>
       <c r="G70">
-        <v>19.579999999999998</v>
+        <v>12.86</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -2710,7 +2712,7 @@
         <v>203</v>
       </c>
       <c r="G73">
-        <v>10.53</v>
+        <v>15.16</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -2779,7 +2781,7 @@
         <v>203</v>
       </c>
       <c r="G76">
-        <v>16.59</v>
+        <v>17.614999999999998</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
@@ -2848,7 +2850,7 @@
         <v>203</v>
       </c>
       <c r="G79">
-        <v>11.92</v>
+        <v>13.49</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
@@ -2917,7 +2919,7 @@
         <v>203</v>
       </c>
       <c r="G82">
-        <v>12.77</v>
+        <v>17.920000000000002</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -2986,7 +2988,7 @@
         <v>203</v>
       </c>
       <c r="G85">
-        <v>19.62</v>
+        <v>15.594999999999899</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -3055,7 +3057,7 @@
         <v>203</v>
       </c>
       <c r="G88">
-        <v>15.66</v>
+        <v>14.344999999999899</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
@@ -3124,7 +3126,7 @@
         <v>203</v>
       </c>
       <c r="G91">
-        <v>16</v>
+        <v>12.845000000000001</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
@@ -3193,7 +3195,7 @@
         <v>203</v>
       </c>
       <c r="G94">
-        <v>12.27</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
@@ -3262,7 +3264,7 @@
         <v>203</v>
       </c>
       <c r="G97">
-        <v>11.94</v>
+        <v>19.350000000000001</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
@@ -3331,7 +3333,7 @@
         <v>203</v>
       </c>
       <c r="G100">
-        <v>18.41</v>
+        <v>12.81</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
@@ -3400,7 +3402,7 @@
         <v>203</v>
       </c>
       <c r="G103">
-        <v>15.57</v>
+        <v>14.71</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
@@ -3469,7 +3471,7 @@
         <v>203</v>
       </c>
       <c r="G106">
-        <v>18.37</v>
+        <v>18.079999999999998</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
@@ -3538,7 +3540,7 @@
         <v>203</v>
       </c>
       <c r="G109">
-        <v>18.22</v>
+        <v>15.654999999999999</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
@@ -3607,7 +3609,7 @@
         <v>203</v>
       </c>
       <c r="G112">
-        <v>11.74</v>
+        <v>17.085000000000001</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
@@ -3676,7 +3678,7 @@
         <v>203</v>
       </c>
       <c r="G115">
-        <v>14.96</v>
+        <v>15.465</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
@@ -3745,7 +3747,7 @@
         <v>203</v>
       </c>
       <c r="G118">
-        <v>13.51</v>
+        <v>14.895</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
@@ -3814,7 +3816,7 @@
         <v>203</v>
       </c>
       <c r="G121">
-        <v>14.24</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
@@ -3883,7 +3885,7 @@
         <v>203</v>
       </c>
       <c r="G124">
-        <v>11.2</v>
+        <v>15.195</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
@@ -3952,7 +3954,7 @@
         <v>203</v>
       </c>
       <c r="G127">
-        <v>18.21</v>
+        <v>15.98</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
@@ -4021,7 +4023,7 @@
         <v>203</v>
       </c>
       <c r="G130">
-        <v>13.73</v>
+        <v>13.455</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
@@ -4090,7 +4092,7 @@
         <v>203</v>
       </c>
       <c r="G133">
-        <v>16.25</v>
+        <v>13.055</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
@@ -4159,7 +4161,7 @@
         <v>203</v>
       </c>
       <c r="G136">
-        <v>16.850000000000001</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
@@ -4228,7 +4230,7 @@
         <v>203</v>
       </c>
       <c r="G139">
-        <v>12.85</v>
+        <v>14.395</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
@@ -4297,7 +4299,7 @@
         <v>203</v>
       </c>
       <c r="G142">
-        <v>10.77</v>
+        <v>12.43</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
@@ -4366,7 +4368,7 @@
         <v>203</v>
       </c>
       <c r="G145">
-        <v>15.8</v>
+        <v>17.375</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
@@ -4435,7 +4437,7 @@
         <v>203</v>
       </c>
       <c r="G148">
-        <v>17.46</v>
+        <v>14.33</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
@@ -4504,7 +4506,7 @@
         <v>203</v>
       </c>
       <c r="G151">
-        <v>18.68</v>
+        <v>17.745000000000001</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
@@ -4573,7 +4575,7 @@
         <v>203</v>
       </c>
       <c r="G154">
-        <v>18.670000000000002</v>
+        <v>14.855</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
@@ -4642,7 +4644,7 @@
         <v>203</v>
       </c>
       <c r="G157">
-        <v>16.11</v>
+        <v>15.035</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
@@ -4711,7 +4713,7 @@
         <v>203</v>
       </c>
       <c r="G160">
-        <v>18.29</v>
+        <v>16.12</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.35">
@@ -4780,7 +4782,7 @@
         <v>203</v>
       </c>
       <c r="G163">
-        <v>14.07</v>
+        <v>14.28</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.35">
@@ -4849,7 +4851,7 @@
         <v>203</v>
       </c>
       <c r="G166">
-        <v>19.670000000000002</v>
+        <v>16.28</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.35">
@@ -4918,7 +4920,7 @@
         <v>203</v>
       </c>
       <c r="G169">
-        <v>10.75</v>
+        <v>15.645</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.35">
@@ -4987,7 +4989,7 @@
         <v>203</v>
       </c>
       <c r="G172">
-        <v>13.76</v>
+        <v>16.47</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.35">
@@ -5056,7 +5058,7 @@
         <v>203</v>
       </c>
       <c r="G175">
-        <v>16.87</v>
+        <v>16.43</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.35">
@@ -5125,7 +5127,7 @@
         <v>203</v>
       </c>
       <c r="G178">
-        <v>12.33</v>
+        <v>12.58</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.35">
@@ -5194,7 +5196,7 @@
         <v>203</v>
       </c>
       <c r="G181">
-        <v>14.27</v>
+        <v>17.805</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.35">
@@ -5263,7 +5265,7 @@
         <v>203</v>
       </c>
       <c r="G184">
-        <v>19.920000000000002</v>
+        <v>15.205</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.35">
@@ -5332,7 +5334,7 @@
         <v>203</v>
       </c>
       <c r="G187">
-        <v>14.35</v>
+        <v>16.914999999999999</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.35">
@@ -5401,7 +5403,7 @@
         <v>203</v>
       </c>
       <c r="G190">
-        <v>17.87</v>
+        <v>15.93</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.35">
@@ -5470,7 +5472,7 @@
         <v>203</v>
       </c>
       <c r="G193">
-        <v>16.05</v>
+        <v>17.43</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.35">
@@ -5539,7 +5541,7 @@
         <v>203</v>
       </c>
       <c r="G196">
-        <v>14.53</v>
+        <v>12.425000000000001</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.35">
@@ -5608,7 +5610,7 @@
         <v>203</v>
       </c>
       <c r="G199">
-        <v>12.63</v>
+        <v>16.754999999999999</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.35">
@@ -5677,7 +5679,7 @@
         <v>203</v>
       </c>
       <c r="G202">
-        <v>11.48</v>
+        <v>15.675000000000001</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.35">
@@ -5746,7 +5748,7 @@
         <v>203</v>
       </c>
       <c r="G205">
-        <v>17.23</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.35">
@@ -5815,7 +5817,7 @@
         <v>203</v>
       </c>
       <c r="G208">
-        <v>13.49</v>
+        <v>12.324999999999999</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.35">
@@ -5884,7 +5886,7 @@
         <v>203</v>
       </c>
       <c r="G211">
-        <v>11.2</v>
+        <v>12.344999999999899</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.35">
@@ -5953,7 +5955,7 @@
         <v>203</v>
       </c>
       <c r="G214">
-        <v>15.78</v>
+        <v>12.675000000000001</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.35">
@@ -6022,7 +6024,7 @@
         <v>203</v>
       </c>
       <c r="G217">
-        <v>18.8</v>
+        <v>14.04</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.35">
@@ -6091,7 +6093,7 @@
         <v>203</v>
       </c>
       <c r="G220">
-        <v>17.57</v>
+        <v>11.239999999999901</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.35">
@@ -6160,7 +6162,7 @@
         <v>203</v>
       </c>
       <c r="G223">
-        <v>17.309999999999999</v>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.35">
@@ -6229,7 +6231,7 @@
         <v>203</v>
       </c>
       <c r="G226">
-        <v>12.44</v>
+        <v>17.524999999999999</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.35">
@@ -6298,7 +6300,7 @@
         <v>203</v>
       </c>
       <c r="G229">
-        <v>17.440000000000001</v>
+        <v>17.16</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.35">
@@ -6367,7 +6369,7 @@
         <v>203</v>
       </c>
       <c r="G232">
-        <v>17.84</v>
+        <v>16.244999999999902</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.35">
@@ -6436,7 +6438,7 @@
         <v>203</v>
       </c>
       <c r="G235">
-        <v>17.63</v>
+        <v>15.125</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.35">
@@ -6505,7 +6507,7 @@
         <v>203</v>
       </c>
       <c r="G238">
-        <v>15.42</v>
+        <v>16.684999999999999</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.35">
@@ -6574,7 +6576,7 @@
         <v>203</v>
       </c>
       <c r="G241">
-        <v>11.91</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.35">
@@ -6643,7 +6645,7 @@
         <v>203</v>
       </c>
       <c r="G244">
-        <v>14.77</v>
+        <v>13.34</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.35">
@@ -6712,7 +6714,7 @@
         <v>203</v>
       </c>
       <c r="G247">
-        <v>17.7</v>
+        <v>10.654999999999999</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.35">
@@ -6781,7 +6783,7 @@
         <v>203</v>
       </c>
       <c r="G250">
-        <v>16.87</v>
+        <v>19.384999999999899</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.35">
@@ -6850,7 +6852,7 @@
         <v>203</v>
       </c>
       <c r="G253">
-        <v>10.210000000000001</v>
+        <v>12.055</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.35">
@@ -6919,7 +6921,7 @@
         <v>203</v>
       </c>
       <c r="G256">
-        <v>19.91</v>
+        <v>18.405000000000001</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.35">
@@ -6988,7 +6990,7 @@
         <v>203</v>
       </c>
       <c r="G259">
-        <v>13.92</v>
+        <v>14.49</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.35">
@@ -7057,7 +7059,7 @@
         <v>203</v>
       </c>
       <c r="G262">
-        <v>13.03</v>
+        <v>15.09</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.35">
@@ -7126,7 +7128,7 @@
         <v>203</v>
       </c>
       <c r="G265">
-        <v>11.2</v>
+        <v>15.145</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.35">
@@ -7195,7 +7197,7 @@
         <v>203</v>
       </c>
       <c r="G268">
-        <v>19.649999999999999</v>
+        <v>19.11</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.35">
@@ -7264,7 +7266,7 @@
         <v>203</v>
       </c>
       <c r="G271">
-        <v>13.02</v>
+        <v>17.895</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.35">
@@ -7333,7 +7335,7 @@
         <v>203</v>
       </c>
       <c r="G274">
-        <v>16.73</v>
+        <v>12.204999999999901</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.35">
@@ -7402,7 +7404,7 @@
         <v>203</v>
       </c>
       <c r="G277">
-        <v>19.38</v>
+        <v>12.344999999999899</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.35">
@@ -7471,7 +7473,7 @@
         <v>203</v>
       </c>
       <c r="G280">
-        <v>16.38</v>
+        <v>14.29</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.35">
@@ -7540,7 +7542,7 @@
         <v>203</v>
       </c>
       <c r="G283">
-        <v>10.82</v>
+        <v>15.87</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.35">
@@ -7609,7 +7611,7 @@
         <v>203</v>
       </c>
       <c r="G286">
-        <v>19.48</v>
+        <v>17.64</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.35">
@@ -7678,7 +7680,7 @@
         <v>203</v>
       </c>
       <c r="G289">
-        <v>12.4</v>
+        <v>12.234999999999999</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.35">
@@ -7747,7 +7749,7 @@
         <v>203</v>
       </c>
       <c r="G292">
-        <v>12.98</v>
+        <v>18.335000000000001</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.35">
@@ -7816,7 +7818,7 @@
         <v>203</v>
       </c>
       <c r="G295">
-        <v>19.8</v>
+        <v>16.38</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.35">
@@ -7885,7 +7887,7 @@
         <v>203</v>
       </c>
       <c r="G298">
-        <v>15.66</v>
+        <v>16.434999999999999</v>
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.35">
@@ -7954,7 +7956,7 @@
         <v>203</v>
       </c>
       <c r="G301">
-        <v>14.85</v>
+        <v>14.64</v>
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.35">
@@ -8023,7 +8025,7 @@
         <v>203</v>
       </c>
       <c r="G304">
-        <v>16.04</v>
+        <v>14.744999999999999</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.35">
@@ -8092,7 +8094,7 @@
         <v>203</v>
       </c>
       <c r="G307">
-        <v>18.54</v>
+        <v>17.420000000000002</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.35">
@@ -8161,7 +8163,7 @@
         <v>203</v>
       </c>
       <c r="G310">
-        <v>14.36</v>
+        <v>15.955</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.35">
@@ -8230,7 +8232,7 @@
         <v>203</v>
       </c>
       <c r="G313">
-        <v>10.39</v>
+        <v>14.93</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.35">
@@ -8299,7 +8301,7 @@
         <v>203</v>
       </c>
       <c r="G316">
-        <v>11.7</v>
+        <v>14.024999999999901</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.35">
@@ -8368,7 +8370,7 @@
         <v>203</v>
       </c>
       <c r="G319">
-        <v>16.79</v>
+        <v>16.305</v>
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.35">
@@ -8437,7 +8439,7 @@
         <v>203</v>
       </c>
       <c r="G322">
-        <v>17.8</v>
+        <v>16.234999999999999</v>
       </c>
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.35">
@@ -8506,7 +8508,7 @@
         <v>203</v>
       </c>
       <c r="G325">
-        <v>18.62</v>
+        <v>15.01</v>
       </c>
     </row>
     <row r="326" spans="1:7" x14ac:dyDescent="0.35">
@@ -8575,7 +8577,7 @@
         <v>203</v>
       </c>
       <c r="G328">
-        <v>10.56</v>
+        <v>15.68</v>
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.35">
@@ -8644,7 +8646,7 @@
         <v>203</v>
       </c>
       <c r="G331">
-        <v>17.71</v>
+        <v>14.445</v>
       </c>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.35">
@@ -8713,7 +8715,7 @@
         <v>203</v>
       </c>
       <c r="G334">
-        <v>15.59</v>
+        <v>15.58</v>
       </c>
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.35">
@@ -8782,7 +8784,7 @@
         <v>203</v>
       </c>
       <c r="G337">
-        <v>10.24</v>
+        <v>13.1299999999999</v>
       </c>
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.35">
@@ -8851,7 +8853,7 @@
         <v>203</v>
       </c>
       <c r="G340">
-        <v>12.88</v>
+        <v>15.425000000000001</v>
       </c>
     </row>
     <row r="341" spans="1:7" x14ac:dyDescent="0.35">
@@ -8920,7 +8922,7 @@
         <v>203</v>
       </c>
       <c r="G343">
-        <v>10.49</v>
+        <v>16.84</v>
       </c>
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.35">
@@ -8989,7 +8991,7 @@
         <v>203</v>
       </c>
       <c r="G346">
-        <v>18.510000000000002</v>
+        <v>14.86</v>
       </c>
     </row>
     <row r="347" spans="1:7" x14ac:dyDescent="0.35">
@@ -9058,7 +9060,7 @@
         <v>203</v>
       </c>
       <c r="G349">
-        <v>15.92</v>
+        <v>12.5049999999999</v>
       </c>
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.35">
@@ -9127,7 +9129,7 @@
         <v>203</v>
       </c>
       <c r="G352">
-        <v>17.47</v>
+        <v>15.545</v>
       </c>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.35">
@@ -9196,7 +9198,7 @@
         <v>203</v>
       </c>
       <c r="G355">
-        <v>16.57</v>
+        <v>13.335000000000001</v>
       </c>
     </row>
     <row r="356" spans="1:7" x14ac:dyDescent="0.35">
@@ -9265,7 +9267,7 @@
         <v>203</v>
       </c>
       <c r="G358">
-        <v>14.9</v>
+        <v>14.52</v>
       </c>
     </row>
     <row r="359" spans="1:7" x14ac:dyDescent="0.35">
@@ -9334,7 +9336,7 @@
         <v>203</v>
       </c>
       <c r="G361">
-        <v>18.82</v>
+        <v>15.04</v>
       </c>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.35">
@@ -9403,7 +9405,7 @@
         <v>203</v>
       </c>
       <c r="G364">
-        <v>18.04</v>
+        <v>17.324999999999999</v>
       </c>
     </row>
     <row r="365" spans="1:7" x14ac:dyDescent="0.35">
@@ -9472,7 +9474,7 @@
         <v>203</v>
       </c>
       <c r="G367">
-        <v>11.9</v>
+        <v>14.074999999999999</v>
       </c>
     </row>
     <row r="368" spans="1:7" x14ac:dyDescent="0.35">
@@ -9541,7 +9543,7 @@
         <v>203</v>
       </c>
       <c r="G370">
-        <v>10.67</v>
+        <v>15.82</v>
       </c>
     </row>
     <row r="371" spans="1:7" x14ac:dyDescent="0.35">
@@ -9610,7 +9612,7 @@
         <v>203</v>
       </c>
       <c r="G373">
-        <v>15.99</v>
+        <v>14.835000000000001</v>
       </c>
     </row>
     <row r="374" spans="1:7" x14ac:dyDescent="0.35">
@@ -9679,7 +9681,7 @@
         <v>203</v>
       </c>
       <c r="G376">
-        <v>10.44</v>
+        <v>17.564999999999898</v>
       </c>
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.35">
@@ -9748,7 +9750,7 @@
         <v>203</v>
       </c>
       <c r="G379">
-        <v>13.37</v>
+        <v>19.795000000000002</v>
       </c>
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.35">
@@ -9817,7 +9819,7 @@
         <v>203</v>
       </c>
       <c r="G382">
-        <v>13.21</v>
+        <v>18.695</v>
       </c>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.35">
@@ -9886,7 +9888,7 @@
         <v>203</v>
       </c>
       <c r="G385">
-        <v>12.35</v>
+        <v>11.824999999999999</v>
       </c>
     </row>
     <row r="386" spans="1:7" x14ac:dyDescent="0.35">
@@ -9955,7 +9957,7 @@
         <v>203</v>
       </c>
       <c r="G388">
-        <v>16.12</v>
+        <v>15.69</v>
       </c>
     </row>
     <row r="389" spans="1:7" x14ac:dyDescent="0.35">
@@ -10024,7 +10026,7 @@
         <v>203</v>
       </c>
       <c r="G391">
-        <v>16.36</v>
+        <v>14.48</v>
       </c>
     </row>
     <row r="392" spans="1:7" x14ac:dyDescent="0.35">
@@ -10093,7 +10095,7 @@
         <v>203</v>
       </c>
       <c r="G394">
-        <v>18.100000000000001</v>
+        <v>18.004999999999999</v>
       </c>
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.35">
@@ -10162,7 +10164,7 @@
         <v>203</v>
       </c>
       <c r="G397">
-        <v>19.38</v>
+        <v>15.18</v>
       </c>
     </row>
     <row r="398" spans="1:7" x14ac:dyDescent="0.35">
@@ -10231,7 +10233,7 @@
         <v>203</v>
       </c>
       <c r="G400">
-        <v>14.57</v>
+        <v>18.22</v>
       </c>
     </row>
     <row r="401" spans="1:7" x14ac:dyDescent="0.35">
@@ -10300,7 +10302,7 @@
         <v>203</v>
       </c>
       <c r="G403">
-        <v>19.809999999999999</v>
+        <v>15.41</v>
       </c>
     </row>
     <row r="404" spans="1:7" x14ac:dyDescent="0.35">
@@ -10369,7 +10371,7 @@
         <v>203</v>
       </c>
       <c r="G406">
-        <v>15.25</v>
+        <v>16.864999999999998</v>
       </c>
     </row>
     <row r="407" spans="1:7" x14ac:dyDescent="0.35">
@@ -10438,7 +10440,7 @@
         <v>203</v>
       </c>
       <c r="G409">
-        <v>17.78</v>
+        <v>16.355</v>
       </c>
     </row>
     <row r="410" spans="1:7" x14ac:dyDescent="0.35">
@@ -10507,7 +10509,7 @@
         <v>203</v>
       </c>
       <c r="G412">
-        <v>19.829999999999998</v>
+        <v>15.53</v>
       </c>
     </row>
     <row r="413" spans="1:7" x14ac:dyDescent="0.35">
@@ -10576,7 +10578,7 @@
         <v>203</v>
       </c>
       <c r="G415">
-        <v>10.52</v>
+        <v>14.315</v>
       </c>
     </row>
     <row r="416" spans="1:7" x14ac:dyDescent="0.35">
@@ -10645,7 +10647,7 @@
         <v>203</v>
       </c>
       <c r="G418">
-        <v>12.81</v>
+        <v>13.42</v>
       </c>
     </row>
     <row r="419" spans="1:7" x14ac:dyDescent="0.35">
@@ -10714,7 +10716,7 @@
         <v>203</v>
       </c>
       <c r="G421">
-        <v>18.96</v>
+        <v>14.535</v>
       </c>
     </row>
     <row r="422" spans="1:7" x14ac:dyDescent="0.35">
@@ -10783,7 +10785,7 @@
         <v>203</v>
       </c>
       <c r="G424">
-        <v>11.4</v>
+        <v>13.315</v>
       </c>
     </row>
     <row r="425" spans="1:7" x14ac:dyDescent="0.35">
@@ -10852,7 +10854,7 @@
         <v>203</v>
       </c>
       <c r="G427">
-        <v>10.199999999999999</v>
+        <v>15.21</v>
       </c>
     </row>
     <row r="428" spans="1:7" x14ac:dyDescent="0.35">
@@ -10921,7 +10923,7 @@
         <v>203</v>
       </c>
       <c r="G430">
-        <v>12.03</v>
+        <v>17.63</v>
       </c>
     </row>
     <row r="431" spans="1:7" x14ac:dyDescent="0.35">
@@ -10990,7 +10992,7 @@
         <v>203</v>
       </c>
       <c r="G433">
-        <v>11.74</v>
+        <v>17.71</v>
       </c>
     </row>
     <row r="434" spans="1:7" x14ac:dyDescent="0.35">
@@ -11059,7 +11061,7 @@
         <v>203</v>
       </c>
       <c r="G436">
-        <v>15</v>
+        <v>14.08</v>
       </c>
     </row>
     <row r="437" spans="1:7" x14ac:dyDescent="0.35">
@@ -11128,7 +11130,7 @@
         <v>203</v>
       </c>
       <c r="G439">
-        <v>14.02</v>
+        <v>14.04</v>
       </c>
     </row>
     <row r="440" spans="1:7" x14ac:dyDescent="0.35">
@@ -11197,7 +11199,7 @@
         <v>203</v>
       </c>
       <c r="G442">
-        <v>18.38</v>
+        <v>14.68</v>
       </c>
     </row>
     <row r="443" spans="1:7" x14ac:dyDescent="0.35">
@@ -11266,7 +11268,7 @@
         <v>203</v>
       </c>
       <c r="G445">
-        <v>16.89</v>
+        <v>15.145</v>
       </c>
     </row>
     <row r="446" spans="1:7" x14ac:dyDescent="0.35">
@@ -11335,7 +11337,7 @@
         <v>203</v>
       </c>
       <c r="G448">
-        <v>19.43</v>
+        <v>13.9749999999999</v>
       </c>
     </row>
     <row r="449" spans="1:7" x14ac:dyDescent="0.35">
@@ -11404,7 +11406,7 @@
         <v>203</v>
       </c>
       <c r="G451">
-        <v>18.05</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="452" spans="1:7" x14ac:dyDescent="0.35">
@@ -11473,7 +11475,7 @@
         <v>203</v>
       </c>
       <c r="G454">
-        <v>14.55</v>
+        <v>17.625</v>
       </c>
     </row>
     <row r="455" spans="1:7" x14ac:dyDescent="0.35">
@@ -11542,7 +11544,7 @@
         <v>203</v>
       </c>
       <c r="G457">
-        <v>10.45</v>
+        <v>14.734999999999999</v>
       </c>
     </row>
     <row r="458" spans="1:7" x14ac:dyDescent="0.35">
@@ -11611,7 +11613,7 @@
         <v>203</v>
       </c>
       <c r="G460">
-        <v>19.66</v>
+        <v>12.125</v>
       </c>
     </row>
     <row r="461" spans="1:7" x14ac:dyDescent="0.35">
@@ -11680,7 +11682,7 @@
         <v>203</v>
       </c>
       <c r="G463">
-        <v>18.329999999999998</v>
+        <v>13.805</v>
       </c>
     </row>
     <row r="464" spans="1:7" x14ac:dyDescent="0.35">
@@ -11749,7 +11751,7 @@
         <v>203</v>
       </c>
       <c r="G466">
-        <v>19.29</v>
+        <v>16.954999999999998</v>
       </c>
     </row>
     <row r="467" spans="1:7" x14ac:dyDescent="0.35">
@@ -11818,7 +11820,7 @@
         <v>203</v>
       </c>
       <c r="G469">
-        <v>17.05</v>
+        <v>12.475</v>
       </c>
     </row>
     <row r="470" spans="1:7" x14ac:dyDescent="0.35">
@@ -11887,7 +11889,7 @@
         <v>203</v>
       </c>
       <c r="G472">
-        <v>13.41</v>
+        <v>19.57</v>
       </c>
     </row>
     <row r="473" spans="1:7" x14ac:dyDescent="0.35">
@@ -11956,7 +11958,7 @@
         <v>203</v>
       </c>
       <c r="G475">
-        <v>19.64</v>
+        <v>14.105</v>
       </c>
     </row>
     <row r="476" spans="1:7" x14ac:dyDescent="0.35">
@@ -12025,7 +12027,7 @@
         <v>203</v>
       </c>
       <c r="G478">
-        <v>19.899999999999999</v>
+        <v>15.53</v>
       </c>
     </row>
     <row r="479" spans="1:7" x14ac:dyDescent="0.35">
@@ -12094,7 +12096,7 @@
         <v>203</v>
       </c>
       <c r="G481">
-        <v>19.48</v>
+        <v>14.239999999999901</v>
       </c>
     </row>
     <row r="482" spans="1:7" x14ac:dyDescent="0.35">
@@ -12163,7 +12165,7 @@
         <v>203</v>
       </c>
       <c r="G484">
-        <v>11.19</v>
+        <v>14.92</v>
       </c>
     </row>
     <row r="485" spans="1:7" x14ac:dyDescent="0.35">
@@ -12232,7 +12234,7 @@
         <v>203</v>
       </c>
       <c r="G487">
-        <v>18.23</v>
+        <v>16.28</v>
       </c>
     </row>
     <row r="488" spans="1:7" x14ac:dyDescent="0.35">
@@ -12301,7 +12303,7 @@
         <v>203</v>
       </c>
       <c r="G490">
-        <v>18.190000000000001</v>
+        <v>14.605</v>
       </c>
     </row>
     <row r="491" spans="1:7" x14ac:dyDescent="0.35">
@@ -12370,7 +12372,7 @@
         <v>203</v>
       </c>
       <c r="G493">
-        <v>16.190000000000001</v>
+        <v>14.945</v>
       </c>
     </row>
     <row r="494" spans="1:7" x14ac:dyDescent="0.35">
@@ -12439,7 +12441,7 @@
         <v>203</v>
       </c>
       <c r="G496">
-        <v>12.32</v>
+        <v>14.55</v>
       </c>
     </row>
     <row r="497" spans="1:7" x14ac:dyDescent="0.35">
@@ -12508,7 +12510,7 @@
         <v>203</v>
       </c>
       <c r="G499">
-        <v>19.010000000000002</v>
+        <v>15.42</v>
       </c>
     </row>
     <row r="500" spans="1:7" x14ac:dyDescent="0.35">
@@ -12577,7 +12579,7 @@
         <v>203</v>
       </c>
       <c r="G502">
-        <v>16.5</v>
+        <v>15.8799999999999</v>
       </c>
     </row>
     <row r="503" spans="1:7" x14ac:dyDescent="0.35">
@@ -12646,7 +12648,7 @@
         <v>203</v>
       </c>
       <c r="G505">
-        <v>14.18</v>
+        <v>15.744999999999999</v>
       </c>
     </row>
     <row r="506" spans="1:7" x14ac:dyDescent="0.35">
@@ -12715,7 +12717,7 @@
         <v>203</v>
       </c>
       <c r="G508">
-        <v>12.2</v>
+        <v>14.385</v>
       </c>
     </row>
     <row r="509" spans="1:7" x14ac:dyDescent="0.35">
@@ -12784,7 +12786,7 @@
         <v>203</v>
       </c>
       <c r="G511">
-        <v>11.45</v>
+        <v>16.664999999999999</v>
       </c>
     </row>
     <row r="512" spans="1:7" x14ac:dyDescent="0.35">
@@ -12853,7 +12855,7 @@
         <v>203</v>
       </c>
       <c r="G514">
-        <v>14.05</v>
+        <v>14.225</v>
       </c>
     </row>
     <row r="515" spans="1:7" x14ac:dyDescent="0.35">
@@ -12922,7 +12924,7 @@
         <v>203</v>
       </c>
       <c r="G517">
-        <v>14.17</v>
+        <v>11.664999999999999</v>
       </c>
     </row>
     <row r="518" spans="1:7" x14ac:dyDescent="0.35">
@@ -12991,7 +12993,7 @@
         <v>203</v>
       </c>
       <c r="G520">
-        <v>10.16</v>
+        <v>12.824999999999999</v>
       </c>
     </row>
     <row r="521" spans="1:7" x14ac:dyDescent="0.35">
@@ -13060,7 +13062,7 @@
         <v>203</v>
       </c>
       <c r="G523">
-        <v>12.75</v>
+        <v>18.145</v>
       </c>
     </row>
     <row r="524" spans="1:7" x14ac:dyDescent="0.35">
@@ -13129,7 +13131,7 @@
         <v>203</v>
       </c>
       <c r="G526">
-        <v>14.04</v>
+        <v>12.51</v>
       </c>
     </row>
     <row r="527" spans="1:7" x14ac:dyDescent="0.35">
@@ -13198,7 +13200,7 @@
         <v>203</v>
       </c>
       <c r="G529">
-        <v>14.88</v>
+        <v>16.71</v>
       </c>
     </row>
     <row r="530" spans="1:7" x14ac:dyDescent="0.35">
@@ -13267,7 +13269,7 @@
         <v>203</v>
       </c>
       <c r="G532">
-        <v>12.69</v>
+        <v>11.51</v>
       </c>
     </row>
     <row r="533" spans="1:7" x14ac:dyDescent="0.35">
@@ -13336,7 +13338,7 @@
         <v>203</v>
       </c>
       <c r="G535">
-        <v>18.690000000000001</v>
+        <v>18.645</v>
       </c>
     </row>
     <row r="536" spans="1:7" x14ac:dyDescent="0.35">
@@ -13405,7 +13407,7 @@
         <v>203</v>
       </c>
       <c r="G538">
-        <v>16.59</v>
+        <v>14.184999999999899</v>
       </c>
     </row>
     <row r="539" spans="1:7" x14ac:dyDescent="0.35">
@@ -13474,7 +13476,7 @@
         <v>203</v>
       </c>
       <c r="G541">
-        <v>13.68</v>
+        <v>18.809999999999999</v>
       </c>
     </row>
     <row r="542" spans="1:7" x14ac:dyDescent="0.35">
@@ -13543,7 +13545,7 @@
         <v>203</v>
       </c>
       <c r="G544">
-        <v>16.940000000000001</v>
+        <v>14.309999999999899</v>
       </c>
     </row>
     <row r="545" spans="1:7" x14ac:dyDescent="0.35">
@@ -13612,7 +13614,7 @@
         <v>203</v>
       </c>
       <c r="G547">
-        <v>11.83</v>
+        <v>13.365</v>
       </c>
     </row>
     <row r="548" spans="1:7" x14ac:dyDescent="0.35">
@@ -13681,7 +13683,7 @@
         <v>203</v>
       </c>
       <c r="G550">
-        <v>12.29</v>
+        <v>17.63</v>
       </c>
     </row>
     <row r="551" spans="1:7" x14ac:dyDescent="0.35">
@@ -13750,7 +13752,7 @@
         <v>203</v>
       </c>
       <c r="G553">
-        <v>11.94</v>
+        <v>13.664999999999999</v>
       </c>
     </row>
     <row r="554" spans="1:7" x14ac:dyDescent="0.35">
@@ -13819,7 +13821,7 @@
         <v>203</v>
       </c>
       <c r="G556">
-        <v>12.11</v>
+        <v>15.52</v>
       </c>
     </row>
     <row r="557" spans="1:7" x14ac:dyDescent="0.35">
@@ -13888,7 +13890,7 @@
         <v>203</v>
       </c>
       <c r="G559">
-        <v>19.27</v>
+        <v>14.855</v>
       </c>
     </row>
     <row r="560" spans="1:7" x14ac:dyDescent="0.35">
@@ -13957,7 +13959,7 @@
         <v>203</v>
       </c>
       <c r="G562">
-        <v>12.73</v>
+        <v>13.395</v>
       </c>
     </row>
     <row r="563" spans="1:7" x14ac:dyDescent="0.35">
@@ -14026,7 +14028,7 @@
         <v>203</v>
       </c>
       <c r="G565">
-        <v>12.9</v>
+        <v>15.89</v>
       </c>
     </row>
     <row r="566" spans="1:7" x14ac:dyDescent="0.35">
@@ -14095,7 +14097,7 @@
         <v>203</v>
       </c>
       <c r="G568">
-        <v>13.68</v>
+        <v>18.574999999999999</v>
       </c>
     </row>
     <row r="569" spans="1:7" x14ac:dyDescent="0.35">
@@ -14164,7 +14166,7 @@
         <v>203</v>
       </c>
       <c r="G571">
-        <v>18.940000000000001</v>
+        <v>11.744999999999999</v>
       </c>
     </row>
     <row r="572" spans="1:7" x14ac:dyDescent="0.35">
@@ -14233,7 +14235,7 @@
         <v>203</v>
       </c>
       <c r="G574">
-        <v>15.46</v>
+        <v>16.484999999999999</v>
       </c>
     </row>
     <row r="575" spans="1:7" x14ac:dyDescent="0.35">
@@ -14302,7 +14304,7 @@
         <v>203</v>
       </c>
       <c r="G577">
-        <v>10.61</v>
+        <v>17.89</v>
       </c>
     </row>
     <row r="578" spans="1:7" x14ac:dyDescent="0.35">
@@ -14371,7 +14373,7 @@
         <v>203</v>
       </c>
       <c r="G580">
-        <v>15.84</v>
+        <v>15.664999999999999</v>
       </c>
     </row>
     <row r="581" spans="1:7" x14ac:dyDescent="0.35">
@@ -14440,7 +14442,7 @@
         <v>203</v>
       </c>
       <c r="G583">
-        <v>15.5</v>
+        <v>15.215</v>
       </c>
     </row>
     <row r="584" spans="1:7" x14ac:dyDescent="0.35">
@@ -14509,7 +14511,7 @@
         <v>203</v>
       </c>
       <c r="G586">
-        <v>14.62</v>
+        <v>17.78</v>
       </c>
     </row>
     <row r="587" spans="1:7" x14ac:dyDescent="0.35">
@@ -14578,7 +14580,7 @@
         <v>203</v>
       </c>
       <c r="G589">
-        <v>15.48</v>
+        <v>11.33</v>
       </c>
     </row>
     <row r="590" spans="1:7" x14ac:dyDescent="0.35">
@@ -14647,7 +14649,7 @@
         <v>203</v>
       </c>
       <c r="G592">
-        <v>14.53</v>
+        <v>17.850000000000001</v>
       </c>
     </row>
     <row r="593" spans="1:7" x14ac:dyDescent="0.35">
@@ -14716,7 +14718,7 @@
         <v>203</v>
       </c>
       <c r="G595">
-        <v>15.53</v>
+        <v>16.004999999999999</v>
       </c>
     </row>
     <row r="596" spans="1:7" x14ac:dyDescent="0.35">
@@ -14785,7 +14787,7 @@
         <v>203</v>
       </c>
       <c r="G598">
-        <v>11.57</v>
+        <v>15.484999999999999</v>
       </c>
     </row>
     <row r="599" spans="1:7" x14ac:dyDescent="0.35">
@@ -14854,7 +14856,7 @@
         <v>203</v>
       </c>
       <c r="G601">
-        <v>19.510000000000002</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="602" spans="1:7" x14ac:dyDescent="0.35">
@@ -14923,7 +14925,7 @@
         <v>203</v>
       </c>
       <c r="G604">
-        <v>13.33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="605" spans="1:7" x14ac:dyDescent="0.35">
@@ -14992,7 +14994,7 @@
         <v>203</v>
       </c>
       <c r="G607">
-        <v>17.329999999999998</v>
+        <v>13.515000000000001</v>
       </c>
     </row>
     <row r="608" spans="1:7" x14ac:dyDescent="0.35">
@@ -15061,7 +15063,7 @@
         <v>203</v>
       </c>
       <c r="G610">
-        <v>15.78</v>
+        <v>15.98</v>
       </c>
     </row>
     <row r="611" spans="1:7" x14ac:dyDescent="0.35">
@@ -15130,7 +15132,7 @@
         <v>203</v>
       </c>
       <c r="G613">
-        <v>11.97</v>
+        <v>16.774999999999999</v>
       </c>
     </row>
     <row r="614" spans="1:7" x14ac:dyDescent="0.35">
@@ -15199,7 +15201,7 @@
         <v>203</v>
       </c>
       <c r="G616">
-        <v>14.94</v>
+        <v>15.64</v>
       </c>
     </row>
     <row r="617" spans="1:7" x14ac:dyDescent="0.35">
@@ -15268,7 +15270,7 @@
         <v>203</v>
       </c>
       <c r="G619">
-        <v>13.85</v>
+        <v>11.065</v>
       </c>
     </row>
     <row r="620" spans="1:7" x14ac:dyDescent="0.35">
@@ -15337,7 +15339,7 @@
         <v>203</v>
       </c>
       <c r="G622">
-        <v>14.44</v>
+        <v>16.119999999999902</v>
       </c>
     </row>
     <row r="623" spans="1:7" x14ac:dyDescent="0.35">
@@ -15406,7 +15408,7 @@
         <v>203</v>
       </c>
       <c r="G625">
-        <v>12.99</v>
+        <v>18.445</v>
       </c>
     </row>
     <row r="626" spans="1:7" x14ac:dyDescent="0.35">
@@ -15475,7 +15477,7 @@
         <v>203</v>
       </c>
       <c r="G628">
-        <v>16.82</v>
+        <v>14.315</v>
       </c>
     </row>
     <row r="629" spans="1:7" x14ac:dyDescent="0.35">
@@ -15544,7 +15546,7 @@
         <v>203</v>
       </c>
       <c r="G631">
-        <v>12.55</v>
+        <v>16.189999999999898</v>
       </c>
     </row>
     <row r="632" spans="1:7" x14ac:dyDescent="0.35">
@@ -15613,7 +15615,7 @@
         <v>203</v>
       </c>
       <c r="G634">
-        <v>19.739999999999998</v>
+        <v>14.03</v>
       </c>
     </row>
     <row r="635" spans="1:7" x14ac:dyDescent="0.35">
@@ -15682,7 +15684,7 @@
         <v>203</v>
       </c>
       <c r="G637">
-        <v>15.13</v>
+        <v>19.369999999999902</v>
       </c>
     </row>
     <row r="638" spans="1:7" x14ac:dyDescent="0.35">
@@ -15751,7 +15753,7 @@
         <v>203</v>
       </c>
       <c r="G640">
-        <v>10.73</v>
+        <v>14.904999999999999</v>
       </c>
     </row>
     <row r="641" spans="1:7" x14ac:dyDescent="0.35">
@@ -15820,7 +15822,7 @@
         <v>203</v>
       </c>
       <c r="G643">
-        <v>12.81</v>
+        <v>14.914999999999999</v>
       </c>
     </row>
     <row r="644" spans="1:7" x14ac:dyDescent="0.35">
@@ -15889,7 +15891,7 @@
         <v>203</v>
       </c>
       <c r="G646">
-        <v>19.13</v>
+        <v>14.989999999999901</v>
       </c>
     </row>
     <row r="647" spans="1:7" x14ac:dyDescent="0.35">
@@ -15958,7 +15960,7 @@
         <v>203</v>
       </c>
       <c r="G649">
-        <v>10.79</v>
+        <v>14.81</v>
       </c>
     </row>
     <row r="650" spans="1:7" x14ac:dyDescent="0.35">
@@ -16027,7 +16029,7 @@
         <v>203</v>
       </c>
       <c r="G652">
-        <v>12.74</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="653" spans="1:7" x14ac:dyDescent="0.35">
@@ -16096,7 +16098,7 @@
         <v>203</v>
       </c>
       <c r="G655">
-        <v>15.71</v>
+        <v>14.365</v>
       </c>
     </row>
     <row r="656" spans="1:7" x14ac:dyDescent="0.35">
@@ -16165,7 +16167,7 @@
         <v>203</v>
       </c>
       <c r="G658">
-        <v>19.260000000000002</v>
+        <v>17.704999999999998</v>
       </c>
     </row>
     <row r="659" spans="1:7" x14ac:dyDescent="0.35">
@@ -16234,7 +16236,7 @@
         <v>203</v>
       </c>
       <c r="G661">
-        <v>13.28</v>
+        <v>14.82</v>
       </c>
     </row>
     <row r="662" spans="1:7" x14ac:dyDescent="0.35">
@@ -16303,7 +16305,7 @@
         <v>203</v>
       </c>
       <c r="G664">
-        <v>18.239999999999998</v>
+        <v>13.855</v>
       </c>
     </row>
     <row r="665" spans="1:7" x14ac:dyDescent="0.35">
@@ -16372,7 +16374,7 @@
         <v>203</v>
       </c>
       <c r="G667">
-        <v>14.28</v>
+        <v>13.19</v>
       </c>
     </row>
     <row r="668" spans="1:7" x14ac:dyDescent="0.35">
@@ -16441,7 +16443,7 @@
         <v>203</v>
       </c>
       <c r="G670">
-        <v>11.42</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="671" spans="1:7" x14ac:dyDescent="0.35">
@@ -16510,7 +16512,7 @@
         <v>203</v>
       </c>
       <c r="G673">
-        <v>17.62</v>
+        <v>13.78</v>
       </c>
     </row>
     <row r="674" spans="1:7" x14ac:dyDescent="0.35">
@@ -16579,7 +16581,7 @@
         <v>203</v>
       </c>
       <c r="G676">
-        <v>14.44</v>
+        <v>13.74</v>
       </c>
     </row>
     <row r="677" spans="1:7" x14ac:dyDescent="0.35">
@@ -16648,7 +16650,7 @@
         <v>203</v>
       </c>
       <c r="G679">
-        <v>10.029999999999999</v>
+        <v>14.48</v>
       </c>
     </row>
     <row r="680" spans="1:7" x14ac:dyDescent="0.35">
@@ -16717,7 +16719,7 @@
         <v>203</v>
       </c>
       <c r="G682">
-        <v>15.04</v>
+        <v>18.055</v>
       </c>
     </row>
     <row r="683" spans="1:7" x14ac:dyDescent="0.35">
@@ -16786,7 +16788,7 @@
         <v>203</v>
       </c>
       <c r="G685">
-        <v>15.08</v>
+        <v>14.43</v>
       </c>
     </row>
     <row r="686" spans="1:7" x14ac:dyDescent="0.35">
@@ -16855,7 +16857,7 @@
         <v>203</v>
       </c>
       <c r="G688">
-        <v>13.95</v>
+        <v>14.215</v>
       </c>
     </row>
     <row r="689" spans="1:7" x14ac:dyDescent="0.35">
@@ -16924,7 +16926,7 @@
         <v>203</v>
       </c>
       <c r="G691">
-        <v>15.82</v>
+        <v>15.9199999999999</v>
       </c>
     </row>
     <row r="692" spans="1:7" x14ac:dyDescent="0.35">
@@ -16993,7 +16995,7 @@
         <v>203</v>
       </c>
       <c r="G694">
-        <v>12.28</v>
+        <v>13.154999999999999</v>
       </c>
     </row>
     <row r="695" spans="1:7" x14ac:dyDescent="0.35">
@@ -17062,7 +17064,7 @@
         <v>203</v>
       </c>
       <c r="G697">
-        <v>10.91</v>
+        <v>16.059999999999999</v>
       </c>
     </row>
     <row r="698" spans="1:7" x14ac:dyDescent="0.35">
@@ -17131,7 +17133,7 @@
         <v>203</v>
       </c>
       <c r="G700">
-        <v>19.98</v>
+        <v>12.96</v>
       </c>
     </row>
     <row r="701" spans="1:7" x14ac:dyDescent="0.35">
@@ -17200,7 +17202,7 @@
         <v>203</v>
       </c>
       <c r="G703">
-        <v>16.25</v>
+        <v>13.455</v>
       </c>
     </row>
     <row r="704" spans="1:7" x14ac:dyDescent="0.35">
@@ -17269,7 +17271,7 @@
         <v>203</v>
       </c>
       <c r="G706">
-        <v>10.57</v>
+        <v>15.705</v>
       </c>
     </row>
     <row r="707" spans="1:7" x14ac:dyDescent="0.35">
@@ -17338,7 +17340,7 @@
         <v>203</v>
       </c>
       <c r="G709">
-        <v>19.510000000000002</v>
+        <v>15.93</v>
       </c>
     </row>
     <row r="710" spans="1:7" x14ac:dyDescent="0.35">
@@ -17407,7 +17409,7 @@
         <v>203</v>
       </c>
       <c r="G712">
-        <v>18.440000000000001</v>
+        <v>17.354999999999901</v>
       </c>
     </row>
     <row r="713" spans="1:7" x14ac:dyDescent="0.35">
@@ -17476,7 +17478,7 @@
         <v>203</v>
       </c>
       <c r="G715">
-        <v>12.74</v>
+        <v>14.51</v>
       </c>
     </row>
     <row r="716" spans="1:7" x14ac:dyDescent="0.35">
@@ -17545,7 +17547,7 @@
         <v>203</v>
       </c>
       <c r="G718">
-        <v>14.37</v>
+        <v>16.46</v>
       </c>
     </row>
     <row r="719" spans="1:7" x14ac:dyDescent="0.35">
@@ -17614,7 +17616,7 @@
         <v>203</v>
       </c>
       <c r="G721">
-        <v>12.22</v>
+        <v>16.02</v>
       </c>
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.35">
@@ -17683,7 +17685,7 @@
         <v>203</v>
       </c>
       <c r="G724">
-        <v>17.34</v>
+        <v>15.045</v>
       </c>
     </row>
     <row r="725" spans="1:7" x14ac:dyDescent="0.35">
@@ -17752,7 +17754,7 @@
         <v>203</v>
       </c>
       <c r="G727">
-        <v>13.52</v>
+        <v>12.84</v>
       </c>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.35">
@@ -17821,7 +17823,7 @@
         <v>203</v>
       </c>
       <c r="G730">
-        <v>19.46</v>
+        <v>15.219999999999899</v>
       </c>
     </row>
     <row r="731" spans="1:7" x14ac:dyDescent="0.35">
@@ -17890,7 +17892,7 @@
         <v>203</v>
       </c>
       <c r="G733">
-        <v>13.04</v>
+        <v>17.41</v>
       </c>
     </row>
     <row r="734" spans="1:7" x14ac:dyDescent="0.35">
@@ -17959,7 +17961,7 @@
         <v>203</v>
       </c>
       <c r="G736">
-        <v>12.18</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="737" spans="1:7" x14ac:dyDescent="0.35">
@@ -18028,7 +18030,7 @@
         <v>203</v>
       </c>
       <c r="G739">
-        <v>17.32</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="740" spans="1:7" x14ac:dyDescent="0.35">
@@ -18097,7 +18099,7 @@
         <v>203</v>
       </c>
       <c r="G742">
-        <v>15.14</v>
+        <v>13.715</v>
       </c>
     </row>
     <row r="743" spans="1:7" x14ac:dyDescent="0.35">
@@ -18166,7 +18168,7 @@
         <v>203</v>
       </c>
       <c r="G745">
-        <v>16.86</v>
+        <v>15.164999999999999</v>
       </c>
     </row>
     <row r="746" spans="1:7" x14ac:dyDescent="0.35">
@@ -18235,7 +18237,7 @@
         <v>203</v>
       </c>
       <c r="G748">
-        <v>12.51</v>
+        <v>17.024999999999999</v>
       </c>
     </row>
     <row r="749" spans="1:7" x14ac:dyDescent="0.35">
@@ -18304,7 +18306,7 @@
         <v>203</v>
       </c>
       <c r="G751">
-        <v>13.46</v>
+        <v>14.95</v>
       </c>
     </row>
     <row r="752" spans="1:7" x14ac:dyDescent="0.35">
@@ -18373,7 +18375,7 @@
         <v>203</v>
       </c>
       <c r="G754">
-        <v>19.39</v>
+        <v>16.164999999999999</v>
       </c>
     </row>
     <row r="755" spans="1:7" x14ac:dyDescent="0.35">
@@ -18442,7 +18444,7 @@
         <v>203</v>
       </c>
       <c r="G757">
-        <v>13</v>
+        <v>16.835000000000001</v>
       </c>
     </row>
     <row r="758" spans="1:7" x14ac:dyDescent="0.35">
@@ -18511,7 +18513,7 @@
         <v>203</v>
       </c>
       <c r="G760">
-        <v>15.63</v>
+        <v>16.125</v>
       </c>
     </row>
     <row r="761" spans="1:7" x14ac:dyDescent="0.35">
@@ -18580,7 +18582,7 @@
         <v>203</v>
       </c>
       <c r="G763">
-        <v>14.33</v>
+        <v>16.98</v>
       </c>
     </row>
     <row r="764" spans="1:7" x14ac:dyDescent="0.35">
@@ -18649,7 +18651,7 @@
         <v>203</v>
       </c>
       <c r="G766">
-        <v>12.14</v>
+        <v>17.734999999999999</v>
       </c>
     </row>
     <row r="767" spans="1:7" x14ac:dyDescent="0.35">
@@ -18718,7 +18720,7 @@
         <v>203</v>
       </c>
       <c r="G769">
-        <v>12.86</v>
+        <v>12.739999999999901</v>
       </c>
     </row>
     <row r="770" spans="1:7" x14ac:dyDescent="0.35">
@@ -18787,7 +18789,7 @@
         <v>203</v>
       </c>
       <c r="G772">
-        <v>18.52</v>
+        <v>16.169999999999899</v>
       </c>
     </row>
     <row r="773" spans="1:7" x14ac:dyDescent="0.35">
@@ -18856,7 +18858,7 @@
         <v>203</v>
       </c>
       <c r="G775">
-        <v>16.62</v>
+        <v>12.385</v>
       </c>
     </row>
     <row r="776" spans="1:7" x14ac:dyDescent="0.35">
@@ -18925,7 +18927,7 @@
         <v>203</v>
       </c>
       <c r="G778">
-        <v>15.7</v>
+        <v>17.734999999999999</v>
       </c>
     </row>
     <row r="779" spans="1:7" x14ac:dyDescent="0.35">
@@ -18994,7 +18996,7 @@
         <v>203</v>
       </c>
       <c r="G781">
-        <v>19.25</v>
+        <v>11.04</v>
       </c>
     </row>
     <row r="782" spans="1:7" x14ac:dyDescent="0.35">
@@ -19063,7 +19065,7 @@
         <v>203</v>
       </c>
       <c r="G784">
-        <v>12.33</v>
+        <v>15.605</v>
       </c>
     </row>
     <row r="785" spans="1:7" x14ac:dyDescent="0.35">
@@ -19132,7 +19134,7 @@
         <v>203</v>
       </c>
       <c r="G787">
-        <v>11.29</v>
+        <v>15.595000000000001</v>
       </c>
     </row>
     <row r="788" spans="1:7" x14ac:dyDescent="0.35">
@@ -19201,7 +19203,7 @@
         <v>203</v>
       </c>
       <c r="G790">
-        <v>16.739999999999998</v>
+        <v>15.48</v>
       </c>
     </row>
     <row r="791" spans="1:7" x14ac:dyDescent="0.35">
@@ -19270,7 +19272,7 @@
         <v>203</v>
       </c>
       <c r="G793">
-        <v>11.5</v>
+        <v>11.585000000000001</v>
       </c>
     </row>
     <row r="794" spans="1:7" x14ac:dyDescent="0.35">
@@ -19339,7 +19341,7 @@
         <v>203</v>
       </c>
       <c r="G796">
-        <v>15.1</v>
+        <v>16.844999999999999</v>
       </c>
     </row>
     <row r="797" spans="1:7" x14ac:dyDescent="0.35">
@@ -19408,7 +19410,7 @@
         <v>203</v>
       </c>
       <c r="G799">
-        <v>15.32</v>
+        <v>17.024999999999999</v>
       </c>
     </row>
     <row r="800" spans="1:7" x14ac:dyDescent="0.35">
@@ -19477,7 +19479,7 @@
         <v>203</v>
       </c>
       <c r="G802">
-        <v>16.559999999999999</v>
+        <v>16.495000000000001</v>
       </c>
     </row>
     <row r="803" spans="1:7" x14ac:dyDescent="0.35">
@@ -19546,7 +19548,7 @@
         <v>203</v>
       </c>
       <c r="G805">
-        <v>13.51</v>
+        <v>16.079999999999998</v>
       </c>
     </row>
     <row r="806" spans="1:7" x14ac:dyDescent="0.35">
@@ -19615,7 +19617,7 @@
         <v>203</v>
       </c>
       <c r="G808">
-        <v>17.34</v>
+        <v>12.524999999999901</v>
       </c>
     </row>
     <row r="809" spans="1:7" x14ac:dyDescent="0.35">
@@ -19684,7 +19686,7 @@
         <v>203</v>
       </c>
       <c r="G811">
-        <v>13.19</v>
+        <v>11.99</v>
       </c>
     </row>
     <row r="812" spans="1:7" x14ac:dyDescent="0.35">
@@ -19753,7 +19755,7 @@
         <v>203</v>
       </c>
       <c r="G814">
-        <v>12.83</v>
+        <v>14.82</v>
       </c>
     </row>
     <row r="815" spans="1:7" x14ac:dyDescent="0.35">
@@ -19822,7 +19824,7 @@
         <v>203</v>
       </c>
       <c r="G817">
-        <v>15</v>
+        <v>16.59</v>
       </c>
     </row>
     <row r="818" spans="1:7" x14ac:dyDescent="0.35">
@@ -19891,7 +19893,7 @@
         <v>203</v>
       </c>
       <c r="G820">
-        <v>14.04</v>
+        <v>18.795000000000002</v>
       </c>
     </row>
     <row r="821" spans="1:7" x14ac:dyDescent="0.35">
@@ -19960,7 +19962,7 @@
         <v>203</v>
       </c>
       <c r="G823">
-        <v>18.11</v>
+        <v>13.225</v>
       </c>
     </row>
     <row r="824" spans="1:7" x14ac:dyDescent="0.35">
@@ -20029,7 +20031,7 @@
         <v>203</v>
       </c>
       <c r="G826">
-        <v>17.190000000000001</v>
+        <v>14.34</v>
       </c>
     </row>
     <row r="827" spans="1:7" x14ac:dyDescent="0.35">
@@ -20098,7 +20100,7 @@
         <v>203</v>
       </c>
       <c r="G829">
-        <v>16.45</v>
+        <v>11.265000000000001</v>
       </c>
     </row>
     <row r="830" spans="1:7" x14ac:dyDescent="0.35">
@@ -20167,7 +20169,7 @@
         <v>203</v>
       </c>
       <c r="G832">
-        <v>19.46</v>
+        <v>17.59</v>
       </c>
     </row>
     <row r="833" spans="1:7" x14ac:dyDescent="0.35">
@@ -20236,7 +20238,7 @@
         <v>203</v>
       </c>
       <c r="G835">
-        <v>16.010000000000002</v>
+        <v>15.76</v>
       </c>
     </row>
     <row r="836" spans="1:7" x14ac:dyDescent="0.35">
@@ -20305,7 +20307,7 @@
         <v>203</v>
       </c>
       <c r="G838">
-        <v>14.24</v>
+        <v>15.615</v>
       </c>
     </row>
     <row r="839" spans="1:7" x14ac:dyDescent="0.35">
@@ -20374,7 +20376,7 @@
         <v>203</v>
       </c>
       <c r="G841">
-        <v>15.92</v>
+        <v>15.285</v>
       </c>
     </row>
     <row r="842" spans="1:7" x14ac:dyDescent="0.35">
@@ -20443,7 +20445,7 @@
         <v>203</v>
       </c>
       <c r="G844">
-        <v>10.130000000000001</v>
+        <v>14.71</v>
       </c>
     </row>
     <row r="845" spans="1:7" x14ac:dyDescent="0.35">
@@ -20512,7 +20514,7 @@
         <v>203</v>
       </c>
       <c r="G847">
-        <v>14.23</v>
+        <v>16.170000000000002</v>
       </c>
     </row>
     <row r="848" spans="1:7" x14ac:dyDescent="0.35">
@@ -20581,7 +20583,7 @@
         <v>203</v>
       </c>
       <c r="G850">
-        <v>10.68</v>
+        <v>14.454999999999901</v>
       </c>
     </row>
     <row r="851" spans="1:7" x14ac:dyDescent="0.35">
@@ -20650,7 +20652,7 @@
         <v>203</v>
       </c>
       <c r="G853">
-        <v>11.48</v>
+        <v>19.175000000000001</v>
       </c>
     </row>
     <row r="854" spans="1:7" x14ac:dyDescent="0.35">
@@ -20719,7 +20721,7 @@
         <v>203</v>
       </c>
       <c r="G856">
-        <v>18.88</v>
+        <v>17.854999999999901</v>
       </c>
     </row>
     <row r="857" spans="1:7" x14ac:dyDescent="0.35">
@@ -20788,7 +20790,7 @@
         <v>203</v>
       </c>
       <c r="G859">
-        <v>17.29</v>
+        <v>14.895</v>
       </c>
     </row>
     <row r="860" spans="1:7" x14ac:dyDescent="0.35">
@@ -20857,7 +20859,7 @@
         <v>203</v>
       </c>
       <c r="G862">
-        <v>15.44</v>
+        <v>16.035</v>
       </c>
     </row>
     <row r="863" spans="1:7" x14ac:dyDescent="0.35">
@@ -20926,7 +20928,7 @@
         <v>203</v>
       </c>
       <c r="G865">
-        <v>11.46</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="866" spans="1:7" x14ac:dyDescent="0.35">
@@ -20995,7 +20997,7 @@
         <v>203</v>
       </c>
       <c r="G868">
-        <v>10.25</v>
+        <v>14.375</v>
       </c>
     </row>
     <row r="869" spans="1:7" x14ac:dyDescent="0.35">
@@ -21064,7 +21066,7 @@
         <v>203</v>
       </c>
       <c r="G871">
-        <v>16.87</v>
+        <v>17.77</v>
       </c>
     </row>
     <row r="872" spans="1:7" x14ac:dyDescent="0.35">
@@ -21133,7 +21135,7 @@
         <v>203</v>
       </c>
       <c r="G874">
-        <v>17.3</v>
+        <v>14.484999999999999</v>
       </c>
     </row>
     <row r="875" spans="1:7" x14ac:dyDescent="0.35">
@@ -21202,7 +21204,7 @@
         <v>203</v>
       </c>
       <c r="G877">
-        <v>19.190000000000001</v>
+        <v>13.324999999999999</v>
       </c>
     </row>
     <row r="878" spans="1:7" x14ac:dyDescent="0.35">
@@ -21271,7 +21273,7 @@
         <v>203</v>
       </c>
       <c r="G880">
-        <v>15.47</v>
+        <v>16.010000000000002</v>
       </c>
     </row>
     <row r="881" spans="1:7" x14ac:dyDescent="0.35">
@@ -21340,7 +21342,7 @@
         <v>203</v>
       </c>
       <c r="G883">
-        <v>10.46</v>
+        <v>17.439999999999898</v>
       </c>
     </row>
     <row r="884" spans="1:7" x14ac:dyDescent="0.35">
@@ -21409,7 +21411,7 @@
         <v>203</v>
       </c>
       <c r="G886">
-        <v>15.87</v>
+        <v>19.189999999999898</v>
       </c>
     </row>
     <row r="887" spans="1:7" x14ac:dyDescent="0.35">
@@ -21478,7 +21480,7 @@
         <v>203</v>
       </c>
       <c r="G889">
-        <v>14.83</v>
+        <v>15.3799999999999</v>
       </c>
     </row>
     <row r="890" spans="1:7" x14ac:dyDescent="0.35">
@@ -21547,7 +21549,7 @@
         <v>203</v>
       </c>
       <c r="G892">
-        <v>18.3</v>
+        <v>15.074999999999999</v>
       </c>
     </row>
     <row r="893" spans="1:7" x14ac:dyDescent="0.35">
@@ -21616,7 +21618,7 @@
         <v>203</v>
       </c>
       <c r="G895">
-        <v>18.350000000000001</v>
+        <v>11.094999999999899</v>
       </c>
     </row>
     <row r="896" spans="1:7" x14ac:dyDescent="0.35">
@@ -21685,7 +21687,7 @@
         <v>203</v>
       </c>
       <c r="G898">
-        <v>10.79</v>
+        <v>13.574999999999999</v>
       </c>
     </row>
     <row r="899" spans="1:7" x14ac:dyDescent="0.35">
@@ -21754,7 +21756,7 @@
         <v>203</v>
       </c>
       <c r="G901">
-        <v>19.48</v>
+        <v>16.89</v>
       </c>
     </row>
     <row r="902" spans="1:7" x14ac:dyDescent="0.35">
@@ -21823,7 +21825,7 @@
         <v>203</v>
       </c>
       <c r="G904">
-        <v>18.28</v>
+        <v>13.98</v>
       </c>
     </row>
     <row r="905" spans="1:7" x14ac:dyDescent="0.35">
@@ -21892,7 +21894,7 @@
         <v>203</v>
       </c>
       <c r="G907">
-        <v>13.85</v>
+        <v>14.32</v>
       </c>
     </row>
     <row r="908" spans="1:7" x14ac:dyDescent="0.35">
@@ -21961,7 +21963,7 @@
         <v>203</v>
       </c>
       <c r="G910">
-        <v>18.79</v>
+        <v>16.32</v>
       </c>
     </row>
     <row r="911" spans="1:7" x14ac:dyDescent="0.35">
@@ -22030,7 +22032,7 @@
         <v>203</v>
       </c>
       <c r="G913">
-        <v>19.88</v>
+        <v>12.835000000000001</v>
       </c>
     </row>
     <row r="914" spans="1:7" x14ac:dyDescent="0.35">
@@ -22099,7 +22101,7 @@
         <v>203</v>
       </c>
       <c r="G916">
-        <v>10.36</v>
+        <v>16.204999999999998</v>
       </c>
     </row>
     <row r="917" spans="1:7" x14ac:dyDescent="0.35">
@@ -22168,7 +22170,7 @@
         <v>203</v>
       </c>
       <c r="G919">
-        <v>19.39</v>
+        <v>17.285</v>
       </c>
     </row>
     <row r="920" spans="1:7" x14ac:dyDescent="0.35">
@@ -22237,7 +22239,7 @@
         <v>203</v>
       </c>
       <c r="G922">
-        <v>15.91</v>
+        <v>14.594999999999899</v>
       </c>
     </row>
     <row r="923" spans="1:7" x14ac:dyDescent="0.35">
@@ -22306,7 +22308,7 @@
         <v>203</v>
       </c>
       <c r="G925">
-        <v>12.83</v>
+        <v>15.285</v>
       </c>
     </row>
     <row r="926" spans="1:7" x14ac:dyDescent="0.35">
@@ -22375,7 +22377,7 @@
         <v>203</v>
       </c>
       <c r="G928">
-        <v>17.77</v>
+        <v>16.149999999999999</v>
       </c>
     </row>
     <row r="929" spans="1:7" x14ac:dyDescent="0.35">
@@ -22444,7 +22446,7 @@
         <v>203</v>
       </c>
       <c r="G931">
-        <v>11.35</v>
+        <v>14.66</v>
       </c>
     </row>
     <row r="932" spans="1:7" x14ac:dyDescent="0.35">
@@ -22513,7 +22515,7 @@
         <v>203</v>
       </c>
       <c r="G934">
-        <v>18.05</v>
+        <v>13.86</v>
       </c>
     </row>
     <row r="935" spans="1:7" x14ac:dyDescent="0.35">
@@ -22582,7 +22584,7 @@
         <v>203</v>
       </c>
       <c r="G937">
-        <v>16.350000000000001</v>
+        <v>16.055</v>
       </c>
     </row>
     <row r="938" spans="1:7" x14ac:dyDescent="0.35">
@@ -22651,7 +22653,7 @@
         <v>203</v>
       </c>
       <c r="G940">
-        <v>12.79</v>
+        <v>10.645</v>
       </c>
     </row>
     <row r="941" spans="1:7" x14ac:dyDescent="0.35">
@@ -22720,7 +22722,7 @@
         <v>203</v>
       </c>
       <c r="G943">
-        <v>17.739999999999998</v>
+        <v>14.07</v>
       </c>
     </row>
     <row r="944" spans="1:7" x14ac:dyDescent="0.35">
@@ -22789,7 +22791,7 @@
         <v>203</v>
       </c>
       <c r="G946">
-        <v>12.7</v>
+        <v>15.965</v>
       </c>
     </row>
     <row r="947" spans="1:7" x14ac:dyDescent="0.35">
@@ -22858,7 +22860,7 @@
         <v>203</v>
       </c>
       <c r="G949">
-        <v>13.29</v>
+        <v>13.845000000000001</v>
       </c>
     </row>
     <row r="950" spans="1:7" x14ac:dyDescent="0.35">
@@ -22927,7 +22929,7 @@
         <v>203</v>
       </c>
       <c r="G952">
-        <v>16.62</v>
+        <v>14.18</v>
       </c>
     </row>
     <row r="953" spans="1:7" x14ac:dyDescent="0.35">
@@ -22996,7 +22998,7 @@
         <v>203</v>
       </c>
       <c r="G955">
-        <v>12.78</v>
+        <v>17.14</v>
       </c>
     </row>
     <row r="956" spans="1:7" x14ac:dyDescent="0.35">
@@ -23065,7 +23067,7 @@
         <v>203</v>
       </c>
       <c r="G958">
-        <v>10.029999999999999</v>
+        <v>15.03</v>
       </c>
     </row>
     <row r="959" spans="1:7" x14ac:dyDescent="0.35">
@@ -23134,7 +23136,7 @@
         <v>203</v>
       </c>
       <c r="G961">
-        <v>12.58</v>
+        <v>14.04</v>
       </c>
     </row>
     <row r="962" spans="1:7" x14ac:dyDescent="0.35">
@@ -23203,7 +23205,7 @@
         <v>203</v>
       </c>
       <c r="G964">
-        <v>15.45</v>
+        <v>16.850000000000001</v>
       </c>
     </row>
     <row r="965" spans="1:7" x14ac:dyDescent="0.35">
@@ -23272,7 +23274,7 @@
         <v>203</v>
       </c>
       <c r="G967">
-        <v>10.86</v>
+        <v>13.86</v>
       </c>
     </row>
     <row r="968" spans="1:7" x14ac:dyDescent="0.35">
@@ -23341,7 +23343,7 @@
         <v>203</v>
       </c>
       <c r="G970">
-        <v>11.06</v>
+        <v>15.925000000000001</v>
       </c>
     </row>
     <row r="971" spans="1:7" x14ac:dyDescent="0.35">
@@ -23410,7 +23412,7 @@
         <v>203</v>
       </c>
       <c r="G973">
-        <v>11.37</v>
+        <v>16.975000000000001</v>
       </c>
     </row>
     <row r="974" spans="1:7" x14ac:dyDescent="0.35">
@@ -23479,7 +23481,7 @@
         <v>203</v>
       </c>
       <c r="G976">
-        <v>18.510000000000002</v>
+        <v>15.73</v>
       </c>
     </row>
     <row r="977" spans="1:7" x14ac:dyDescent="0.35">
@@ -23548,7 +23550,7 @@
         <v>203</v>
       </c>
       <c r="G979">
-        <v>16.96</v>
+        <v>14.675000000000001</v>
       </c>
     </row>
     <row r="980" spans="1:7" x14ac:dyDescent="0.35">
@@ -23617,7 +23619,7 @@
         <v>203</v>
       </c>
       <c r="G982">
-        <v>10.31</v>
+        <v>15.895</v>
       </c>
     </row>
     <row r="983" spans="1:7" x14ac:dyDescent="0.35">
@@ -23686,7 +23688,7 @@
         <v>203</v>
       </c>
       <c r="G985">
-        <v>11.44</v>
+        <v>18.920000000000002</v>
       </c>
     </row>
     <row r="986" spans="1:7" x14ac:dyDescent="0.35">
@@ -23755,7 +23757,7 @@
         <v>203</v>
       </c>
       <c r="G988">
-        <v>17.100000000000001</v>
+        <v>12.719999999999899</v>
       </c>
     </row>
     <row r="989" spans="1:7" x14ac:dyDescent="0.35">
@@ -23824,7 +23826,7 @@
         <v>203</v>
       </c>
       <c r="G991">
-        <v>16.53</v>
+        <v>16.57</v>
       </c>
     </row>
     <row r="992" spans="1:7" x14ac:dyDescent="0.35">
@@ -23893,7 +23895,7 @@
         <v>203</v>
       </c>
       <c r="G994">
-        <v>17.5</v>
+        <v>16.314999999999898</v>
       </c>
     </row>
     <row r="995" spans="1:7" x14ac:dyDescent="0.35">
@@ -23962,7 +23964,7 @@
         <v>203</v>
       </c>
       <c r="G997">
-        <v>16.670000000000002</v>
+        <v>11.705</v>
       </c>
     </row>
     <row r="998" spans="1:7" x14ac:dyDescent="0.35">
@@ -24031,7 +24033,7 @@
         <v>203</v>
       </c>
       <c r="G1000">
-        <v>11.3</v>
+        <v>13.445</v>
       </c>
     </row>
     <row r="1001" spans="1:7" x14ac:dyDescent="0.35">
@@ -24100,7 +24102,7 @@
         <v>203</v>
       </c>
       <c r="G1003">
-        <v>17.86</v>
+        <v>14.175000000000001</v>
       </c>
     </row>
     <row r="1004" spans="1:7" x14ac:dyDescent="0.35">
@@ -24169,7 +24171,7 @@
         <v>203</v>
       </c>
       <c r="G1006">
-        <v>11.85</v>
+        <v>16.704999999999998</v>
       </c>
     </row>
     <row r="1007" spans="1:7" x14ac:dyDescent="0.35">
@@ -24238,7 +24240,7 @@
         <v>203</v>
       </c>
       <c r="G1009">
-        <v>18.14</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="1010" spans="1:7" x14ac:dyDescent="0.35">
@@ -24307,7 +24309,7 @@
         <v>203</v>
       </c>
       <c r="G1012">
-        <v>10.68</v>
+        <v>18.035</v>
       </c>
     </row>
     <row r="1013" spans="1:7" x14ac:dyDescent="0.35">
@@ -24376,7 +24378,7 @@
         <v>203</v>
       </c>
       <c r="G1015">
-        <v>15.75</v>
+        <v>13.324999999999999</v>
       </c>
     </row>
     <row r="1016" spans="1:7" x14ac:dyDescent="0.35">
@@ -24445,7 +24447,7 @@
         <v>203</v>
       </c>
       <c r="G1018">
-        <v>10.28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="1019" spans="1:7" x14ac:dyDescent="0.35">
@@ -24514,7 +24516,7 @@
         <v>203</v>
       </c>
       <c r="G1021">
-        <v>15.33</v>
+        <v>14.85</v>
       </c>
     </row>
     <row r="1022" spans="1:7" x14ac:dyDescent="0.35">
@@ -24583,7 +24585,7 @@
         <v>203</v>
       </c>
       <c r="G1024">
-        <v>15.45</v>
+        <v>17.73</v>
       </c>
     </row>
     <row r="1025" spans="1:7" x14ac:dyDescent="0.35">
@@ -24652,7 +24654,7 @@
         <v>203</v>
       </c>
       <c r="G1027">
-        <v>16.29</v>
+        <v>12.71</v>
       </c>
     </row>
     <row r="1028" spans="1:7" x14ac:dyDescent="0.35">
@@ -24721,7 +24723,7 @@
         <v>203</v>
       </c>
       <c r="G1030">
-        <v>18.12</v>
+        <v>15.494999999999999</v>
       </c>
     </row>
     <row r="1031" spans="1:7" x14ac:dyDescent="0.35">
@@ -24790,7 +24792,7 @@
         <v>203</v>
       </c>
       <c r="G1033">
-        <v>10.119999999999999</v>
+        <v>12.185</v>
       </c>
     </row>
     <row r="1034" spans="1:7" x14ac:dyDescent="0.35">
@@ -24859,7 +24861,7 @@
         <v>203</v>
       </c>
       <c r="G1036">
-        <v>12.49</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="1037" spans="1:7" x14ac:dyDescent="0.35">
@@ -24928,7 +24930,7 @@
         <v>203</v>
       </c>
       <c r="G1039">
-        <v>11.14</v>
+        <v>17.47</v>
       </c>
     </row>
     <row r="1040" spans="1:7" x14ac:dyDescent="0.35">
@@ -24997,7 +24999,7 @@
         <v>203</v>
       </c>
       <c r="G1042">
-        <v>18.420000000000002</v>
+        <v>16.07</v>
       </c>
     </row>
     <row r="1043" spans="1:7" x14ac:dyDescent="0.35">
@@ -25066,7 +25068,7 @@
         <v>203</v>
       </c>
       <c r="G1045">
-        <v>13.89</v>
+        <v>16.39</v>
       </c>
     </row>
     <row r="1046" spans="1:7" x14ac:dyDescent="0.35">
@@ -25135,7 +25137,7 @@
         <v>203</v>
       </c>
       <c r="G1048">
-        <v>19.059999999999999</v>
+        <v>15.365</v>
       </c>
     </row>
     <row r="1049" spans="1:7" x14ac:dyDescent="0.35">
@@ -25204,7 +25206,7 @@
         <v>203</v>
       </c>
       <c r="G1051">
-        <v>17.010000000000002</v>
+        <v>13.865</v>
       </c>
     </row>
     <row r="1052" spans="1:7" x14ac:dyDescent="0.35">
@@ -25273,7 +25275,7 @@
         <v>203</v>
       </c>
       <c r="G1054">
-        <v>17.579999999999998</v>
+        <v>16.285</v>
       </c>
     </row>
     <row r="1055" spans="1:7" x14ac:dyDescent="0.35">
@@ -25342,7 +25344,7 @@
         <v>203</v>
       </c>
       <c r="G1057">
-        <v>13.25</v>
+        <v>14.434999999999899</v>
       </c>
     </row>
     <row r="1058" spans="1:7" x14ac:dyDescent="0.35">
@@ -25411,7 +25413,7 @@
         <v>203</v>
       </c>
       <c r="G1060">
-        <v>13.64</v>
+        <v>14.425000000000001</v>
       </c>
     </row>
     <row r="1061" spans="1:7" x14ac:dyDescent="0.35">
@@ -25480,7 +25482,7 @@
         <v>203</v>
       </c>
       <c r="G1063">
-        <v>16.239999999999998</v>
+        <v>17.549999999999901</v>
       </c>
     </row>
     <row r="1064" spans="1:7" x14ac:dyDescent="0.35">
@@ -25549,7 +25551,7 @@
         <v>203</v>
       </c>
       <c r="G1066">
-        <v>13.6</v>
+        <v>16.510000000000002</v>
       </c>
     </row>
     <row r="1067" spans="1:7" x14ac:dyDescent="0.35">
@@ -25618,7 +25620,7 @@
         <v>203</v>
       </c>
       <c r="G1069">
-        <v>17.66</v>
+        <v>12.64</v>
       </c>
     </row>
     <row r="1070" spans="1:7" x14ac:dyDescent="0.35">
@@ -25687,7 +25689,7 @@
         <v>203</v>
       </c>
       <c r="G1072">
-        <v>17.420000000000002</v>
+        <v>15.225</v>
       </c>
     </row>
     <row r="1073" spans="1:7" x14ac:dyDescent="0.35">
@@ -25756,7 +25758,7 @@
         <v>203</v>
       </c>
       <c r="G1075">
-        <v>11.02</v>
+        <v>17.175000000000001</v>
       </c>
     </row>
     <row r="1076" spans="1:7" x14ac:dyDescent="0.35">
@@ -25825,7 +25827,7 @@
         <v>203</v>
       </c>
       <c r="G1078">
-        <v>19.02</v>
+        <v>16.645</v>
       </c>
     </row>
     <row r="1079" spans="1:7" x14ac:dyDescent="0.35">
@@ -25894,7 +25896,7 @@
         <v>203</v>
       </c>
       <c r="G1081">
-        <v>16.440000000000001</v>
+        <v>13.324999999999999</v>
       </c>
     </row>
     <row r="1082" spans="1:7" x14ac:dyDescent="0.35">
@@ -25963,7 +25965,7 @@
         <v>203</v>
       </c>
       <c r="G1084">
-        <v>16.45</v>
+        <v>15.565</v>
       </c>
     </row>
     <row r="1085" spans="1:7" x14ac:dyDescent="0.35">
@@ -26032,7 +26034,7 @@
         <v>203</v>
       </c>
       <c r="G1087">
-        <v>12.86</v>
+        <v>15.145</v>
       </c>
     </row>
     <row r="1088" spans="1:7" x14ac:dyDescent="0.35">
@@ -26101,7 +26103,7 @@
         <v>203</v>
       </c>
       <c r="G1090">
-        <v>10.52</v>
+        <v>14.33</v>
       </c>
     </row>
     <row r="1091" spans="1:7" x14ac:dyDescent="0.35">
@@ -26170,7 +26172,7 @@
         <v>203</v>
       </c>
       <c r="G1093">
-        <v>12.81</v>
+        <v>17.844999999999999</v>
       </c>
     </row>
     <row r="1094" spans="1:7" x14ac:dyDescent="0.35">
@@ -26239,7 +26241,7 @@
         <v>203</v>
       </c>
       <c r="G1096">
-        <v>11.28</v>
+        <v>12.88</v>
       </c>
     </row>
     <row r="1097" spans="1:7" x14ac:dyDescent="0.35">
@@ -26308,7 +26310,7 @@
         <v>203</v>
       </c>
       <c r="G1099">
-        <v>12</v>
+        <v>14.82</v>
       </c>
     </row>
     <row r="1100" spans="1:7" x14ac:dyDescent="0.35">
@@ -26377,7 +26379,7 @@
         <v>203</v>
       </c>
       <c r="G1102">
-        <v>14.01</v>
+        <v>12.524999999999901</v>
       </c>
     </row>
     <row r="1103" spans="1:7" x14ac:dyDescent="0.35">
@@ -26446,7 +26448,7 @@
         <v>203</v>
       </c>
       <c r="G1105">
-        <v>11.89</v>
+        <v>16.594999999999999</v>
       </c>
     </row>
     <row r="1106" spans="1:7" x14ac:dyDescent="0.35">
@@ -26515,7 +26517,7 @@
         <v>203</v>
       </c>
       <c r="G1108">
-        <v>14.25</v>
+        <v>10.58</v>
       </c>
     </row>
     <row r="1109" spans="1:7" x14ac:dyDescent="0.35">
@@ -26584,7 +26586,7 @@
         <v>203</v>
       </c>
       <c r="G1111">
-        <v>16.84</v>
+        <v>13.8799999999999</v>
       </c>
     </row>
     <row r="1112" spans="1:7" x14ac:dyDescent="0.35">
@@ -26653,7 +26655,7 @@
         <v>203</v>
       </c>
       <c r="G1114">
-        <v>11.7</v>
+        <v>18.375</v>
       </c>
     </row>
     <row r="1115" spans="1:7" x14ac:dyDescent="0.35">
@@ -26722,7 +26724,7 @@
         <v>203</v>
       </c>
       <c r="G1117">
-        <v>14.55</v>
+        <v>15.309999999999899</v>
       </c>
     </row>
     <row r="1118" spans="1:7" x14ac:dyDescent="0.35">
@@ -26791,7 +26793,7 @@
         <v>203</v>
       </c>
       <c r="G1120">
-        <v>12.23</v>
+        <v>15.98</v>
       </c>
     </row>
     <row r="1121" spans="1:7" x14ac:dyDescent="0.35">
@@ -26860,7 +26862,7 @@
         <v>203</v>
       </c>
       <c r="G1123">
-        <v>11.67</v>
+        <v>13.0049999999999</v>
       </c>
     </row>
     <row r="1124" spans="1:7" x14ac:dyDescent="0.35">
@@ -26929,7 +26931,7 @@
         <v>203</v>
       </c>
       <c r="G1126">
-        <v>15.59</v>
+        <v>16.625</v>
       </c>
     </row>
     <row r="1127" spans="1:7" x14ac:dyDescent="0.35">
@@ -26998,7 +27000,7 @@
         <v>203</v>
       </c>
       <c r="G1129">
-        <v>13.43</v>
+        <v>15.27</v>
       </c>
     </row>
     <row r="1130" spans="1:7" x14ac:dyDescent="0.35">
@@ -27067,7 +27069,7 @@
         <v>203</v>
       </c>
       <c r="G1132">
-        <v>18</v>
+        <v>15.205</v>
       </c>
     </row>
     <row r="1133" spans="1:7" x14ac:dyDescent="0.35">
@@ -27136,7 +27138,7 @@
         <v>203</v>
       </c>
       <c r="G1135">
-        <v>17.53</v>
+        <v>18.739999999999998</v>
       </c>
     </row>
     <row r="1136" spans="1:7" x14ac:dyDescent="0.35">
@@ -27205,7 +27207,7 @@
         <v>203</v>
       </c>
       <c r="G1138">
-        <v>16.62</v>
+        <v>13.64</v>
       </c>
     </row>
     <row r="1139" spans="1:7" x14ac:dyDescent="0.35">
@@ -27274,7 +27276,7 @@
         <v>203</v>
       </c>
       <c r="G1141">
-        <v>16.940000000000001</v>
+        <v>15.125</v>
       </c>
     </row>
     <row r="1142" spans="1:7" x14ac:dyDescent="0.35">
@@ -27343,7 +27345,7 @@
         <v>203</v>
       </c>
       <c r="G1144">
-        <v>17.5</v>
+        <v>11.265000000000001</v>
       </c>
     </row>
     <row r="1145" spans="1:7" x14ac:dyDescent="0.35">
@@ -27412,7 +27414,7 @@
         <v>203</v>
       </c>
       <c r="G1147">
-        <v>11.87</v>
+        <v>14.92</v>
       </c>
     </row>
     <row r="1148" spans="1:7" x14ac:dyDescent="0.35">
@@ -27481,7 +27483,7 @@
         <v>203</v>
       </c>
       <c r="G1150">
-        <v>14.83</v>
+        <v>14.775</v>
       </c>
     </row>
     <row r="1151" spans="1:7" x14ac:dyDescent="0.35">
@@ -27550,7 +27552,7 @@
         <v>203</v>
       </c>
       <c r="G1153">
-        <v>10.79</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="1154" spans="1:7" x14ac:dyDescent="0.35">
@@ -27619,7 +27621,7 @@
         <v>203</v>
       </c>
       <c r="G1156">
-        <v>18.09</v>
+        <v>15.18</v>
       </c>
     </row>
     <row r="1157" spans="1:7" x14ac:dyDescent="0.35">
@@ -27688,7 +27690,7 @@
         <v>203</v>
       </c>
       <c r="G1159">
-        <v>12.02</v>
+        <v>16.63</v>
       </c>
     </row>
     <row r="1160" spans="1:7" x14ac:dyDescent="0.35">
@@ -27757,7 +27759,7 @@
         <v>203</v>
       </c>
       <c r="G1162">
-        <v>10.37</v>
+        <v>14.829999999999901</v>
       </c>
     </row>
     <row r="1163" spans="1:7" x14ac:dyDescent="0.35">
@@ -27826,7 +27828,7 @@
         <v>203</v>
       </c>
       <c r="G1165">
-        <v>15.72</v>
+        <v>17.074999999999999</v>
       </c>
     </row>
     <row r="1166" spans="1:7" x14ac:dyDescent="0.35">
@@ -27895,7 +27897,7 @@
         <v>203</v>
       </c>
       <c r="G1168">
-        <v>10.220000000000001</v>
+        <v>17.13</v>
       </c>
     </row>
     <row r="1169" spans="1:7" x14ac:dyDescent="0.35">
@@ -27964,7 +27966,7 @@
         <v>203</v>
       </c>
       <c r="G1171">
-        <v>19.21</v>
+        <v>17.564999999999898</v>
       </c>
     </row>
     <row r="1172" spans="1:7" x14ac:dyDescent="0.35">
@@ -28033,7 +28035,7 @@
         <v>203</v>
       </c>
       <c r="G1174">
-        <v>14.64</v>
+        <v>14.295</v>
       </c>
     </row>
     <row r="1175" spans="1:7" x14ac:dyDescent="0.35">
@@ -28102,7 +28104,7 @@
         <v>203</v>
       </c>
       <c r="G1177">
-        <v>11.17</v>
+        <v>13.649999999999901</v>
       </c>
     </row>
     <row r="1178" spans="1:7" x14ac:dyDescent="0.35">
@@ -28171,7 +28173,7 @@
         <v>203</v>
       </c>
       <c r="G1180">
-        <v>15.87</v>
+        <v>12.07</v>
       </c>
     </row>
     <row r="1181" spans="1:7" x14ac:dyDescent="0.35">
@@ -28240,7 +28242,7 @@
         <v>203</v>
       </c>
       <c r="G1183">
-        <v>10.88</v>
+        <v>15.37</v>
       </c>
     </row>
     <row r="1184" spans="1:7" x14ac:dyDescent="0.35">
@@ -28309,7 +28311,7 @@
         <v>203</v>
       </c>
       <c r="G1186">
-        <v>13.9</v>
+        <v>18.759999999999899</v>
       </c>
     </row>
     <row r="1187" spans="1:7" x14ac:dyDescent="0.35">
@@ -28378,7 +28380,7 @@
         <v>203</v>
       </c>
       <c r="G1189">
-        <v>16.46</v>
+        <v>11.555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>